<commit_message>
Backup to GitHub - 2021.04.17
</commit_message>
<xml_diff>
--- a/02_Logistic_Regression/Output/InLrPt_00_Results_Summary.xlsx
+++ b/02_Logistic_Regression/Output/InLrPt_00_Results_Summary.xlsx
@@ -847,7 +847,7 @@
         <v>583</v>
       </c>
       <c r="C12">
-        <v>0.286</v>
+        <v>0.714</v>
       </c>
       <c r="D12">
         <v>0.452</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -897,7 +897,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>7.829326445064638</v>
+        <v>8.028118934152998</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -908,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>4.088652864529585</v>
+        <v>4.105928322727145</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>5.479385703522196</v>
+        <v>5.479306339060577</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -930,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>5.779720013727657</v>
+        <v>5.758439174509814</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -941,7 +941,7 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>2.665135003680805</v>
+        <v>2.68855644444936</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -952,7 +952,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>3.326781058914075</v>
+        <v>3.349120513095468</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -963,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>3.193024688499279</v>
+        <v>3.196186622121956</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -974,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>102.235956789184</v>
+        <v>105.7667082703045</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -985,7 +985,7 @@
         <v>16</v>
       </c>
       <c r="C10">
-        <v>133.0557195284925</v>
+        <v>135.4044845455055</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -996,7 +996,7 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>25.91626899772592</v>
+        <v>25.86720161629629</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1007,7 +1007,7 @@
         <v>18</v>
       </c>
       <c r="C12">
-        <v>1.543903166217791</v>
+        <v>3.942859723556538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>